<commit_message>
Worked on CPL files for 12-12 vreg arenas.
</commit_message>
<xml_diff>
--- a/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -142,109 +142,226 @@
     <t xml:space="preserve">C34</t>
   </si>
   <si>
+    <t xml:space="preserve">C35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
     <t xml:space="preserve">J2</t>
   </si>
   <si>
-    <t xml:space="preserve">J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1</t>
+    <t xml:space="preserve">SW1</t>
   </si>
   <si>
     <t xml:space="preserve">P1</t>
@@ -281,9 +398,6 @@
   </si>
   <si>
     <t xml:space="preserve">P12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
   </si>
 </sst>
 </file>
@@ -402,7 +516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,6 +541,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,83 +597,83 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>273.9136</v>
+        <v>106.7905</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-220.5228</v>
+        <v>-287.663</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>287.274</v>
+        <v>94.2705</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-220.472</v>
+        <v>-287.633</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>274.545</v>
+        <v>129.7634</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>-239.08</v>
+        <v>-287.7112</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>286.885</v>
+        <v>117.5134</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>-239.08</v>
+        <v>-287.7312</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>236.69</v>
+        <v>235.9022</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>-293.674</v>
+        <v>-287.6804</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -564,15 +682,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>224.355</v>
+        <v>223.4022</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>-293.684</v>
+        <v>-287.6904</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -581,15 +699,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>274.292</v>
+        <v>259.4102</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>-293.624</v>
+        <v>-287.6804</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -598,15 +716,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>261.912</v>
+        <v>246.6355</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-293.654</v>
+        <v>-287.663</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -615,15 +733,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>192.504</v>
+        <v>174.7142</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>-293.604</v>
+        <v>-287.7312</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -632,15 +750,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>180.354</v>
+        <v>162.1892</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>-293.564</v>
+        <v>-287.8012</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -649,304 +767,304 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>278.704</v>
+        <v>277.3172</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>-202.73</v>
+        <v>-153.0988</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>278.704</v>
+        <v>271.78</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>-189.23</v>
+        <v>-153.1112</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>277.6505</v>
+        <v>269.9512</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>-148.938</v>
+        <v>-154.826</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>270.9005</v>
+        <v>251.6338</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>-137.2467</v>
+        <v>-106.6495</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>249.842</v>
+        <v>246.8447</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>-102.8795</v>
+        <v>-109.4289</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>238.1507</v>
+        <v>246.1183</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>-96.1295</v>
+        <v>-111.8283</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="18" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>202.73</v>
+        <v>206.1667</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>-76.896</v>
+        <v>-79.265</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>189.23</v>
+        <v>203.4089</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>-76.896</v>
+        <v>-84.0665</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="20" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>148.938</v>
+        <v>203.9795</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>-77.9495</v>
+        <v>-86.5077</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>137.2467</v>
+        <v>153.0988</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>-84.6995</v>
+        <v>-78.2828</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>102.8795</v>
+        <v>153.1112</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>-105.758</v>
+        <v>-83.82</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>96.1295</v>
+        <v>154.826</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>-117.4493</v>
+        <v>-85.6488</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>76.896</v>
+        <v>106.6495</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>-152.87</v>
+        <v>-103.9662</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="25" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>76.896</v>
+        <v>109.4289</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>-166.37</v>
+        <v>-108.7553</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>77.9495</v>
+        <v>111.8283</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>-206.662</v>
+        <v>-109.4817</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>84.6995</v>
+        <v>79.265</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>-218.3533</v>
+        <v>-149.4333</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="28" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>105.758</v>
+        <v>84.0665</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>-252.7205</v>
+        <v>-152.1911</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>117.4493</v>
+        <v>86.5077</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>-259.4705</v>
+        <v>-151.6205</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -955,15 +1073,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>152.87</v>
+        <v>78.2828</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>-278.704</v>
+        <v>-202.5012</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
@@ -972,15 +1090,15 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>166.37</v>
+        <v>83.82</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>-278.704</v>
+        <v>-202.4888</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -989,134 +1107,134 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>206.662</v>
+        <v>85.6488</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>-277.6505</v>
+        <v>-200.774</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>218.3533</v>
+        <v>103.9662</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>-270.9005</v>
+        <v>-248.9505</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="34" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>252.7205</v>
+        <v>108.7553</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>-249.842</v>
+        <v>-246.1711</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>259.4705</v>
+        <v>109.4817</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>-238.1507</v>
+        <v>-243.7717</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>301.5</v>
+        <v>149.4333</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>-239.516</v>
+        <v>-276.335</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="37" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>301.5</v>
+        <v>152.1911</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>-230.505</v>
+        <v>-271.5335</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>291.2055</v>
+        <v>151.6205</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>-169.164</v>
+        <v>-269.0923</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>293.2195</v>
+        <v>202.5012</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>-172.466</v>
+        <v>-277.3172</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -1125,32 +1243,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>295.148</v>
+        <v>202.4888</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>-169.164</v>
+        <v>-271.78</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>278.45</v>
+        <v>200.774</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>-184.826</v>
+        <v>-269.9512</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
@@ -1159,202 +1277,202 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>268.4785</v>
+        <v>248.9505</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>-133.5597</v>
+        <v>-251.6338</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>234.2097</v>
+        <v>246.1711</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>-94.1475</v>
+        <v>-246.8447</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="44" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>184.826</v>
+        <v>243.7717</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>-77.15</v>
+        <v>-246.1183</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="45" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>133.5597</v>
+        <v>276.335</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>-87.1215</v>
+        <v>-206.1667</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>94.1475</v>
+        <v>271.5335</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>-121.3903</v>
+        <v>-203.4089</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="47" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>77.15</v>
+        <v>269.0923</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>-170.774</v>
+        <v>-203.9795</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="48" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>87.1215</v>
+        <v>191.1734</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>-222.0403</v>
+        <v>-287.4772</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>121.3903</v>
+        <v>186.8834</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>-261.4525</v>
+        <v>-283.9422</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="50" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>170.774</v>
+        <v>274.32</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>-278.45</v>
+        <v>-160.02</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>222.0403</v>
+        <v>252.4988</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>-268.4785</v>
+        <v>-114.1421</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="52" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>261.4525</v>
+        <v>210.6621</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>-234.2097</v>
+        <v>-85.3212</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="53" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>280.8555</v>
+        <v>160.02</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>-222.799</v>
+        <v>-81.28</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
@@ -1363,292 +1481,270 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>280.7409</v>
+        <v>114.1421</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>-241.3398</v>
+        <v>-103.1012</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="55" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>230.5396</v>
+        <v>85.3212</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>-291.4176</v>
+        <v>-144.9379</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="56" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>267.9826</v>
+        <v>81.28</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>-291.3668</v>
+        <v>-195.58</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>186.5017</v>
+        <v>103.1012</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>-291.2958</v>
+        <v>-241.4579</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>278.659028</v>
+        <v>144.9379</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>-196.003</v>
+        <v>-270.2788</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>180</v>
-      </c>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>274.247981</v>
+        <v>195.58</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>-143.134745</v>
+        <v>-274.32</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>210</v>
-      </c>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>243.993774</v>
+        <v>241.4579</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>-99.555018</v>
+        <v>-252.4988</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>240</v>
-      </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>196.003</v>
+        <v>270.2788</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>-76.940971</v>
+        <v>-210.6621</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>270</v>
-      </c>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>143.134745</v>
+        <v>284.6015</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>-81.352018</v>
+        <v>-127.4064</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>99.555018</v>
+        <v>286.6155</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>-111.606225</v>
+        <v>-130.7084</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>330</v>
-      </c>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>76.940971</v>
+        <v>288.544</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>-159.597</v>
+        <v>-127.4064</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="65" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>81.352018</v>
+        <v>265.9888</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>-212.465254</v>
+        <v>-154.8638</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>111.606225</v>
+        <v>268.0208</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>-256.044981</v>
+        <v>-154.8892</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="67" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>159.597</v>
+        <v>242.7056</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>-278.659028</v>
+        <v>-113.8423</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>212.465254</v>
+        <v>244.4781</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>-274.247981</v>
+        <v>-112.8483</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="69" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>256.044981</v>
+        <v>202.0311</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>-243.993774</v>
+        <v>-89.9582</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -1656,137 +1752,135 @@
       <c r="E69" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>304.6</v>
+        <v>203.0691</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>-116.459</v>
+        <v>-88.2111</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="71" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>265.474</v>
+        <v>154.8638</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>-177.8</v>
+        <v>-89.6112</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>253.7279</v>
+        <v>154.8892</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>-133.963</v>
+        <v>-87.5792</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>221.637</v>
+        <v>113.8423</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>-101.8721</v>
+        <v>-112.8944</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="74" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>177.8</v>
+        <v>112.8483</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>-90.126</v>
+        <v>-111.1219</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>133.963</v>
+        <v>89.9582</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>-101.8721</v>
+        <v>-153.5689</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="76" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>101.8721</v>
+        <v>88.2111</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>-133.963</v>
+        <v>-152.5309</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>90.126</v>
+        <v>89.6112</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>-177.8</v>
+        <v>-200.7362</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>6</v>
@@ -1795,108 +1889,855 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>101.8721</v>
+        <v>87.5792</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>-221.637</v>
+        <v>-200.7108</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>133.963</v>
+        <v>112.8944</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>-253.7279</v>
+        <v>-241.7577</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="80" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B80" s="2" t="n">
-        <v>177.8</v>
+        <v>111.1219</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>-265.474</v>
+        <v>-242.7517</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B81" s="2" t="n">
-        <v>221.637</v>
+        <v>153.5689</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>-253.7279</v>
+        <v>-265.6418</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="82" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B82" s="2" t="n">
-        <v>253.7279</v>
+        <v>152.5309</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>-221.637</v>
+        <v>-267.3889</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B83" s="2" t="n">
-        <v>299.5</v>
+        <v>200.7362</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>-86.233</v>
+        <v>-265.9888</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E83" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>200.7108</v>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>-268.0208</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>241.7577</v>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>-242.7056</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
+      <c r="B86" s="2" t="n">
+        <v>242.7517</v>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>-244.4781</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="87" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>265.6418</v>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>-202.0311</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>267.3889</v>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>-203.0691</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="89" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>100.5155</v>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>-285.373</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>123.7534</v>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>-285.4412</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>229.8072</v>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>-285.4104</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="92" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>252.9155</v>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>-285.373</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>168.5592</v>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>-285.5012</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>274.5384</v>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>-154.2233</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>249.7896</v>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>-109.0128</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>205.7512</v>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>-82.2337</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>154.2233</v>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>-81.0616</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>109.0128</v>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>-105.8104</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="99" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>82.2337</v>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>-149.8488</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="100" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>81.0616</v>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>-201.3767</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="101" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>105.8104</v>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>-246.5872</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="102" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>149.8488</v>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>-273.3663</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="103" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>201.3767</v>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>-274.5384</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>246.5872</v>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>-249.7896</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>273.3663</v>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>-205.7512</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>189.9034</v>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>-284.0847</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>292.0238</v>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>-92.0242</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="108" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>285.75</v>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>-228.6</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>287.02</v>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>-112.0902</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="110" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>266.474</v>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>-177.8</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="111" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>254.594</v>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>-133.463</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="112" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B112" s="2" t="n">
+        <v>222.137</v>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>-101.006</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="113" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>177.8</v>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>-89.126</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>133.463</v>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>-101.006</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B115" s="2" t="n">
+        <v>101.006</v>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>-133.463</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>89.126</v>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>-177.8</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>101.006</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>-222.137</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>133.463</v>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>-254.594</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>177.8</v>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>-266.474</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="120" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>222.137</v>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>-254.594</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="121" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>254.594</v>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>-222.137</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Fixed component rotations in NI 12-12 arena w/ vreg for JLCPCB upload.
</commit_message>
<xml_diff>
--- a/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
@@ -461,7 +461,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +472,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
   </fills>
@@ -516,7 +540,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -545,6 +569,38 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,6 +610,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFF6F9D4"/>
+      <rgbColor rgb="FFDEE6EF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -565,7 +681,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1617,21 +1733,21 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+    <row r="62" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="7" t="n">
         <v>284.6015</v>
       </c>
-      <c r="C62" s="2" t="n">
+      <c r="C62" s="7" t="n">
         <v>-127.4064</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>180</v>
+      <c r="D62" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,310 +2192,310 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="89" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+    <row r="89" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="2" t="n">
+      <c r="B89" s="9" t="n">
         <v>100.5155</v>
       </c>
-      <c r="C89" s="2" t="n">
+      <c r="C89" s="9" t="n">
         <v>-285.373</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E89" s="2" t="n">
+      <c r="D89" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="9" t="n">
+        <v>123.7534</v>
+      </c>
+      <c r="C90" s="9" t="n">
+        <v>-285.4412</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="9" t="n">
+        <v>229.8072</v>
+      </c>
+      <c r="C91" s="9" t="n">
+        <v>-285.4104</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="9" t="n">
+        <v>252.9155</v>
+      </c>
+      <c r="C92" s="9" t="n">
+        <v>-285.373</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="9" t="n">
+        <v>168.5592</v>
+      </c>
+      <c r="C93" s="9" t="n">
+        <v>-285.5012</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="11" t="n">
+        <v>274.5384</v>
+      </c>
+      <c r="C94" s="11" t="n">
+        <v>-154.2233</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="11" t="n">
+        <v>249.7896</v>
+      </c>
+      <c r="C95" s="11" t="n">
+        <v>-109.0128</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="11" t="n">
+        <v>205.7512</v>
+      </c>
+      <c r="C96" s="11" t="n">
+        <v>-82.2337</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="11" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="11" t="n">
+        <v>154.2233</v>
+      </c>
+      <c r="C97" s="11" t="n">
+        <v>-81.0616</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="11" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" s="11" t="n">
+        <v>109.0128</v>
+      </c>
+      <c r="C98" s="11" t="n">
+        <v>-105.8104</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="11" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="11" t="n">
+        <v>82.2337</v>
+      </c>
+      <c r="C99" s="11" t="n">
+        <v>-149.8488</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="11" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="11" t="n">
+        <v>81.0616</v>
+      </c>
+      <c r="C100" s="11" t="n">
+        <v>-201.3767</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="11" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="90" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="2" t="n">
-        <v>123.7534</v>
-      </c>
-      <c r="C90" s="2" t="n">
-        <v>-285.4412</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B91" s="2" t="n">
-        <v>229.8072</v>
-      </c>
-      <c r="C91" s="2" t="n">
-        <v>-285.4104</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="2" t="n">
-        <v>252.9155</v>
-      </c>
-      <c r="C92" s="2" t="n">
-        <v>-285.373</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="93" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B93" s="2" t="n">
-        <v>168.5592</v>
-      </c>
-      <c r="C93" s="2" t="n">
-        <v>-285.5012</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="94" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="2" t="n">
-        <v>274.5384</v>
-      </c>
-      <c r="C94" s="2" t="n">
-        <v>-154.2233</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="95" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B95" s="2" t="n">
-        <v>249.7896</v>
-      </c>
-      <c r="C95" s="2" t="n">
-        <v>-109.0128</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="96" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B96" s="2" t="n">
-        <v>205.7512</v>
-      </c>
-      <c r="C96" s="2" t="n">
-        <v>-82.2337</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="97" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B97" s="2" t="n">
-        <v>154.2233</v>
-      </c>
-      <c r="C97" s="2" t="n">
-        <v>-81.0616</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="98" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B98" s="2" t="n">
-        <v>109.0128</v>
-      </c>
-      <c r="C98" s="2" t="n">
-        <v>-105.8104</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="99" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B99" s="2" t="n">
-        <v>82.2337</v>
-      </c>
-      <c r="C99" s="2" t="n">
-        <v>-149.8488</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="100" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="2" t="n">
-        <v>81.0616</v>
-      </c>
-      <c r="C100" s="2" t="n">
-        <v>-201.3767</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="101" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
+    <row r="101" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="2" t="n">
+      <c r="B101" s="11" t="n">
         <v>105.8104</v>
       </c>
-      <c r="C101" s="2" t="n">
+      <c r="C101" s="11" t="n">
         <v>-246.5872</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="102" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
+      <c r="D101" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="11" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="2" t="n">
+      <c r="B102" s="11" t="n">
         <v>149.8488</v>
       </c>
-      <c r="C102" s="2" t="n">
+      <c r="C102" s="11" t="n">
         <v>-273.3663</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="103" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
+      <c r="D102" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="11" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="103" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B103" s="2" t="n">
+      <c r="B103" s="11" t="n">
         <v>201.3767</v>
       </c>
-      <c r="C103" s="2" t="n">
+      <c r="C103" s="11" t="n">
         <v>-274.5384</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="2" t="n">
+      <c r="D103" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="11" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="104" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" s="11" t="n">
+        <v>246.5872</v>
+      </c>
+      <c r="C104" s="11" t="n">
+        <v>-249.7896</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="11" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="105" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B105" s="11" t="n">
+        <v>273.3663</v>
+      </c>
+      <c r="C105" s="11" t="n">
+        <v>-205.7512</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="11" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="106" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B106" s="13" t="n">
+        <v>189.9034</v>
+      </c>
+      <c r="C106" s="13" t="n">
+        <v>-284.0847</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="13" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="104" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B104" s="2" t="n">
-        <v>246.5872</v>
-      </c>
-      <c r="C104" s="2" t="n">
-        <v>-249.7896</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="105" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B105" s="2" t="n">
-        <v>273.3663</v>
-      </c>
-      <c r="C105" s="2" t="n">
-        <v>-205.7512</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="106" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B106" s="2" t="n">
-        <v>189.9034</v>
-      </c>
-      <c r="C106" s="2" t="n">
-        <v>-284.0847</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>90</v>
       </c>
     </row>
     <row r="107" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Remade gerber files for NI 12-12 vreg arena design.
</commit_message>
<xml_diff>
--- a/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/CPL_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
@@ -680,8 +680,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E109" activeCellId="0" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2529,7 +2529,7 @@
         <v>6</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="109" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>